<commit_message>
Upload final dashboard-only version (no env)
</commit_message>
<xml_diff>
--- a/data/IP_List.xlsx
+++ b/data/IP_List.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cangelop\Desktop\Python\Ping_Dashboard_v2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8F31E4-168B-4ADB-8888-283F2FCBB5A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8695E4C-A614-4D41-AC21-E29DF42B8267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BEFA2C6C-E960-4B91-99A7-53EA4C7F9485}"/>
+    <workbookView xWindow="29580" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{BEFA2C6C-E960-4B91-99A7-53EA4C7F9485}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$123</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="246">
   <si>
     <t>Name</t>
   </si>
@@ -270,30 +273,9 @@
     <t>172.16.6.119</t>
   </si>
   <si>
-    <t>172.16.6.121</t>
-  </si>
-  <si>
-    <t>172.16.6.122</t>
-  </si>
-  <si>
-    <t>172.16.6.123</t>
-  </si>
-  <si>
-    <t>172.16.6.124</t>
-  </si>
-  <si>
     <t>172.16.6.125</t>
   </si>
   <si>
-    <t>172.16.6.128</t>
-  </si>
-  <si>
-    <t>St Leonards Land Main Electricity</t>
-  </si>
-  <si>
-    <t>172.16.6.129</t>
-  </si>
-  <si>
     <t>172.16.6.131</t>
   </si>
   <si>
@@ -339,12 +321,6 @@
     <t>172.16.6.219</t>
   </si>
   <si>
-    <t>172.16.6.220</t>
-  </si>
-  <si>
-    <t>172.16.6.223</t>
-  </si>
-  <si>
     <t>172.16.6.224</t>
   </si>
   <si>
@@ -354,9 +330,6 @@
     <t>172.16.6.230</t>
   </si>
   <si>
-    <t>172.16.6.232</t>
-  </si>
-  <si>
     <t>172.16.6.233</t>
   </si>
   <si>
@@ -381,9 +354,6 @@
     <t>172.16.6.255</t>
   </si>
   <si>
-    <t>172.16.6.44</t>
-  </si>
-  <si>
     <t>172.16.6.45</t>
   </si>
   <si>
@@ -642,24 +612,9 @@
     <t>Minto House Main Electricity Incomer</t>
   </si>
   <si>
-    <t>Pattersons Land Main Electricity No. 1 / No.2</t>
-  </si>
-  <si>
-    <t>Dalhousie Land Main Electricity</t>
-  </si>
-  <si>
-    <t>St Johns Land Main Electricity</t>
-  </si>
-  <si>
-    <t>Simon Laurie House Main Electricity</t>
-  </si>
-  <si>
     <t>Fleming House</t>
   </si>
   <si>
-    <t>ECA Main Building - Electrical Incomer</t>
-  </si>
-  <si>
     <t>ECCI Building</t>
   </si>
   <si>
@@ -705,12 +660,6 @@
     <t>Potterrow - Car Park</t>
   </si>
   <si>
-    <t>Potterrow Basement</t>
-  </si>
-  <si>
-    <t>Adam House - Main Incomer</t>
-  </si>
-  <si>
     <t>Appleton Tower - Basement Switchroom</t>
   </si>
   <si>
@@ -720,9 +669,6 @@
     <t>Main Library - Chiller Plantroom</t>
   </si>
   <si>
-    <t>Informatics</t>
-  </si>
-  <si>
     <t>Dugald Stewart</t>
   </si>
   <si>
@@ -745,9 +691,6 @@
   </si>
   <si>
     <t>St Leonards Land</t>
-  </si>
-  <si>
-    <t>Adam House</t>
   </si>
   <si>
     <t>46 Pleasance - New LV Switchboard</t>
@@ -1209,10 +1152,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C05DA3D-E331-4C1C-A785-FC40DDCEA135}">
-  <dimension ref="A1:B133"/>
+  <dimension ref="A1:B123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A123" sqref="A2:A123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,31 +1174,31 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>261</v>
+        <v>241</v>
       </c>
       <c r="B2" t="s">
-        <v>262</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="B3" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>259</v>
+        <v>239</v>
       </c>
       <c r="B4" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -1263,7 +1206,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -1271,7 +1214,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -1279,7 +1222,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -1287,7 +1230,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -1303,7 +1246,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -1311,15 +1254,15 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="B12" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -1407,7 +1350,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="B24" t="s">
         <v>31</v>
@@ -1415,7 +1358,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="B25" t="s">
         <v>32</v>
@@ -1423,15 +1366,15 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="B26" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="B27" t="s">
         <v>33</v>
@@ -1439,7 +1382,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="B28" t="s">
         <v>34</v>
@@ -1447,7 +1390,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="B29" t="s">
         <v>35</v>
@@ -1455,7 +1398,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="B30" t="s">
         <v>36</v>
@@ -1463,15 +1406,15 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="B31" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>264</v>
+        <v>244</v>
       </c>
       <c r="B32" t="s">
         <v>37</v>
@@ -1487,7 +1430,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="B34" t="s">
         <v>40</v>
@@ -1495,15 +1438,15 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="B35" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="B36" t="s">
         <v>41</v>
@@ -1511,7 +1454,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="B37" t="s">
         <v>42</v>
@@ -1519,7 +1462,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="B38" t="s">
         <v>43</v>
@@ -1527,7 +1470,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B39" t="s">
         <v>44</v>
@@ -1535,15 +1478,15 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="B40" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B41" t="s">
         <v>45</v>
@@ -1551,7 +1494,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B42" t="s">
         <v>46</v>
@@ -1559,7 +1502,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="B43" t="s">
         <v>47</v>
@@ -1567,7 +1510,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="B44" t="s">
         <v>48</v>
@@ -1575,7 +1518,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="B45" t="s">
         <v>49</v>
@@ -1583,7 +1526,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="B46" t="s">
         <v>50</v>
@@ -1591,7 +1534,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="B47" t="s">
         <v>51</v>
@@ -1599,7 +1542,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="B48" t="s">
         <v>52</v>
@@ -1607,7 +1550,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>265</v>
+        <v>245</v>
       </c>
       <c r="B49" t="s">
         <v>53</v>
@@ -1615,15 +1558,15 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="B50" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="B51" t="s">
         <v>54</v>
@@ -1631,7 +1574,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="B52" t="s">
         <v>55</v>
@@ -1639,7 +1582,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="B53" t="s">
         <v>56</v>
@@ -1647,7 +1590,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B54" t="s">
         <v>57</v>
@@ -1655,7 +1598,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B55" t="s">
         <v>58</v>
@@ -1663,7 +1606,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B56" t="s">
         <v>59</v>
@@ -1671,7 +1614,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="B57" t="s">
         <v>60</v>
@@ -1679,7 +1622,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="B58" t="s">
         <v>61</v>
@@ -1687,7 +1630,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="B59" t="s">
         <v>62</v>
@@ -1695,7 +1638,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="B60" t="s">
         <v>63</v>
@@ -1703,7 +1646,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="B61" t="s">
         <v>64</v>
@@ -1711,7 +1654,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B62" t="s">
         <v>65</v>
@@ -1719,7 +1662,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="B63" t="s">
         <v>66</v>
@@ -1727,7 +1670,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="B64" t="s">
         <v>67</v>
@@ -1735,7 +1678,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="B65" t="s">
         <v>68</v>
@@ -1743,7 +1686,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="B66" t="s">
         <v>69</v>
@@ -1751,7 +1694,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="B67" t="s">
         <v>70</v>
@@ -1759,7 +1702,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="B68" t="s">
         <v>71</v>
@@ -1767,7 +1710,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="B69" t="s">
         <v>72</v>
@@ -1775,7 +1718,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="B70" t="s">
         <v>73</v>
@@ -1783,7 +1726,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="B71" t="s">
         <v>74</v>
@@ -1791,7 +1734,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="B72" t="s">
         <v>75</v>
@@ -1799,15 +1742,15 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="B73" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="B74" t="s">
         <v>77</v>
@@ -1815,7 +1758,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="B75" t="s">
         <v>78</v>
@@ -1823,7 +1766,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="B76" t="s">
         <v>79</v>
@@ -1831,7 +1774,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="B77" t="s">
         <v>80</v>
@@ -1839,7 +1782,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="B78" t="s">
         <v>81</v>
@@ -1847,7 +1790,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="B79" t="s">
         <v>82</v>
@@ -1855,7 +1798,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="B80" t="s">
         <v>83</v>
@@ -1863,231 +1806,231 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>197</v>
+      </c>
+      <c r="B81" t="s">
         <v>84</v>
-      </c>
-      <c r="B81" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B82" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="B83" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="B84" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="B85" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="B86" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="B87" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="B88" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="B89" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="B90" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="B91" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="B92" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="B93" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="B94" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="B95" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="B96" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="B97" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="B98" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="B99" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="B100" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="B101" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="B102" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="B103" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="B104" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="B105" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="B106" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="B107" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="B108" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>235</v>
+        <v>112</v>
       </c>
       <c r="B109" t="s">
         <v>113</v>
@@ -2095,7 +2038,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="B110" t="s">
         <v>114</v>
@@ -2103,189 +2046,110 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="B111" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="B112" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="B113" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="B114" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="B115" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="B116" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="B117" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="B118" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>123</v>
+        <v>234</v>
       </c>
       <c r="B119" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="B120" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="B121" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="B122" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="B123" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>249</v>
-      </c>
-      <c r="B124" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>250</v>
-      </c>
-      <c r="B125" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>251</v>
-      </c>
-      <c r="B126" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>252</v>
-      </c>
-      <c r="B127" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>253</v>
-      </c>
-      <c r="B128" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>254</v>
-      </c>
-      <c r="B129" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>255</v>
-      </c>
-      <c r="B130" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>256</v>
-      </c>
-      <c r="B131" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>257</v>
-      </c>
-      <c r="B132" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>258</v>
-      </c>
-      <c r="B133" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B123" xr:uid="{0C05DA3D-E331-4C1C-A785-FC40DDCEA135}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>